<commit_message>
Update overdue rule parsing
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanwyn/Project/qms-monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F102BBFD-3B39-864F-A592-B24E9760BA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{43230C0A-F275-3F46-B640-0112063C6BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="740" windowWidth="28100" windowHeight="17220" xr2:uid="{3B55A8ED-9442-8048-9FD1-0DCD55720AC0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="190" uniqueCount="58">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="191" uniqueCount="59">
   <si>
     <t>序号</t>
   </si>
@@ -208,6 +208,10 @@
   </si>
   <si>
     <t>OOS/OOT-CAPA</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成时限</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1180,15 +1184,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF3A8A3-DB77-5943-9AFF-B7A5D4B60337}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1240,8 +1244,11 @@
       <c r="Q1" t="s">
         <v>52</v>
       </c>
+      <c r="R1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1269,6 +1276,9 @@
       <c r="I2" t="s">
         <v>19</v>
       </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
       <c r="K2" t="s">
         <v>20</v>
       </c>
@@ -1285,7 +1295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1338,7 +1348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1382,7 +1392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1435,7 +1445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1479,7 +1489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1532,7 +1542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1576,7 +1586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1626,7 +1636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1670,7 +1680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1720,7 +1730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1764,7 +1774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1814,7 +1824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1864,7 +1874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>